<commit_message>
Adding Pojo classes for Customer and Customer address Refactoring
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CreateCustomerTestDataExtended.xlsx
+++ b/src/test/resources/testData/CreateCustomerTestDataExtended.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7905"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="TestData" sheetId="4" r:id="rId2"/>
+    <sheet name="TestData" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
-  <si>
-    <t>TestCases</t>
-  </si>
-  <si>
-    <t>RunMode</t>
-  </si>
-  <si>
-    <t>createCustomerWithValidToken</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +75,36 @@
   </si>
   <si>
     <t>+38014881337</t>
+  </si>
+  <si>
+    <t>address[country]</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>address[line2]</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>address[line1]</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>address[postal_code]</t>
+  </si>
+  <si>
+    <t>address[state]</t>
+  </si>
+  <si>
+    <t>Kyiv obl.</t>
+  </si>
+  <si>
+    <t>createCustomerWithValidTokenUsingPojo</t>
   </si>
 </sst>
 </file>
@@ -131,13 +148,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -422,162 +436,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7400</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7400</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>